<commit_message>
commit as of 05/02/2020 -Add guest API, -History search API
</commit_message>
<xml_diff>
--- a/doc/WaitlistAPIListTechRevamp.xlsx
+++ b/doc/WaitlistAPIListTechRevamp.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="112">
   <si>
     <t>API</t>
   </si>
@@ -3508,6 +3508,9 @@
   </si>
   <si>
     <t>client base is need for creating tiny url</t>
+  </si>
+  <si>
+    <t>{"serviceResult":{"NOW_SERVING_GUEST_ID":1,"ORG_TOTAL_WAIT_TIME":24,"NEXT_TO_NOTIFY_GUEST_ID":19513,"OP":"ADD","totalWaitTime":24,"nowServingParty":1,"totalPartiesWaiting":5,"orgid":83,"addedGuestId":19514,"guestUUID":"0910c2d2","tinyURL":"https://tinyurl.com/wamax57#/s/0910c2d2","guestRank":5,"languagePrefID":{"langId":1,"langName":"English","languageDisplayName":null,"langIsoCode":"en","active":false},"partyType":-1}</t>
   </si>
 </sst>
 </file>
@@ -4188,8 +4191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="E14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4454,7 +4457,7 @@
         <v>41</v>
       </c>
       <c r="F14" s="31" t="s">
-        <v>41</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="5" customFormat="1" ht="240" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
- update waitlist API'S response in doc.
</commit_message>
<xml_diff>
--- a/doc/WaitlistAPIListTechRevamp.xlsx
+++ b/doc/WaitlistAPIListTechRevamp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Kyobee11Nov\NewUI branch\RevisedKyobee\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ria\Kyobee\Kyobee\RevisedKyobee\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="118">
   <si>
     <t>API</t>
   </si>
@@ -3319,42 +3319,6 @@
   </si>
   <si>
     <t>orgid,partyType,searchName,pagerReqParam</t>
-  </si>
-  <si>
-    <t>{ "guestID": 19504, "organizationID": 83, "name": "Fagun", "note": null, "uuid": "2d65c97f", "noOfPeople": 1,"partyType": -1, "email": null, "sms": "4242423423", "status": "CHECKIN", "rank": 1, "prefType": "sms","optin": true, "calloutCount": null, "checkinTime": 1580291488000, "seatedTime": null,"createdTime": 1580291649680, "updatedTime": 1580291649680,  "incompleteParty": null, "seatingPreference": [{
-        "prefValueId": 39,
-        "prefValue": "Patio",
-        "prefKey": null
-      }], "marketingPreference": [{
-        "prefValueId": 39,
-        "prefValue": "Patio",
-        "prefKey": null
-      }], "deviceType": null, "deviceId": null, "languagePref": { "langId": 1, "langName": "English", "languageDisplayName": "English", "langIsoCode": "en", "active": true} }</t>
-  </si>
-  <si>
-    <t>"serviceResult": { "totalRecords": 1, "pageNo": 1, "records": [ { "guestID": 19504, "organizationID": 83, "name": "Fagun", "note": null, "uuid": "2d65c97f","noOfPeople": 1, "partyType": -1, "email": null, "sms": "4242423423", "status": "CHECKIN", "rank": 1, "prefType": "sms", "optin": true, "calloutCount": null, "checkinTime": 1580291488000, "seatedTime": null, "createdTime": 1580291649680, "updatedTime": 1580291649680, "incompleteParty": null, "seatingPreference": [{
-        "prefValueId": 39,
-        "prefValue": "Patio",
-        "prefKey": null
-      }], "marketingPreference": [{
-        "prefValueId": 39,
-        "prefValue": "Patio",
-        "prefKey": null
-      }], "deviceType": null, "deviceId": null, "languagePref": { "langId": 1, "langName": "English", "languageDisplayName": "English", "langIsoCode": "en", "active": true} } ] }</t>
-  </si>
-  <si>
-    <t>"serviceResult": { "totalRecords": 1, "pageNo": 1, "records": [ { "guestID": 19504, "organizationID": 83, "name": "Fagun", "note": null, "uuid": "2d65c97f","noOfPeople": 1, "partyType": -1, "email": null, "sms": "4242423423", "status": "CHECKIN", "rank": 1, "prefType": "sms", "optin": true, "calloutCount": null, "checkinTime": 1580291488000, "seatedTime": null, "createdTime": 1580291649680, "updatedTime": 1580291649680, "incompleteParty": null, "seatingPreference": [], "marketingPreference":[], "deviceType": null, "deviceId": null, "languagePref": { "langId": 1, "langName": "English", "languageDisplayName": "English", "langIsoCode": "en", "active": true} } ] }</t>
-  </si>
-  <si>
-    <t>{ "guestID": 19504, "organizationID": 83, "name": "Fagun", "note": null, "uuid": "2d65c97f","noOfPeople": 1, "partyType": -1, "email": null, "sms": "4242423423", "status": "CHECKIN", "rank": 1, "prefType": "sms", "optin": true, "calloutCount": null, "checkinTime": 1580291488000, "seatedTime": null,"incompleteParty": null, "seatingPreference": [{
-        "prefValueId": 39,
-        "prefValue": "Patio",
-        "prefKey": null
-      }], "marketingPreference": [{
-        "prefValueId": 39,
-        "prefValue": "Patio",
-        "prefKey": null
-      }], "languagePrefID": { "langId": 1, "langName": "English", "languageDisplayName": "English", "langIsoCode": "en", "active": true}, "languageMap": { }}</t>
   </si>
   <si>
     <t>{"totalRecords":6,"pageNo":1,"records":[{"guestID":19485,"organizationID":1,"name":"Max 5","note":null,"uuid":"48291306","noOfPeople":3,"partyType":-1,"email":null,"sms":"1212121212","status":"DELETED","rank":5,"prefType":"sms","optin":true,"calloutCount":null,"checkinTime":1580216574000,"seatedTime":null,"incompleteParty":null,"seatingPreference":[],"marketingPreference":[],"deviceType":null,"deviceId":null,"languagePref":{"langId":1,"langName":"English","languageDisplayName":"English","langIsoCode":"en"}]}</t>
@@ -3421,12 +3385,6 @@
     <t>guestId,orgId,status</t>
   </si>
   <si>
-    <t>{"orgid":83,"pageSize":1000,"pageNo":1}</t>
-  </si>
-  <si>
-    <t>{"orgid":83,searchtext:"abc","pageSize":1000,"pageNo":1}</t>
-  </si>
-  <si>
     <t>{clientTimezone: +05:30,
 orgid: 83,
 sliderMaxTime: 24,
@@ -3450,17 +3408,6 @@
   </si>
   <si>
     <t>Doubte(Need to discuss)</t>
-  </si>
-  <si>
-    <t>"serviceResult": {
-    "OP_NOTIFYUSERCOUNT": "2",
-    "ORG_TOTAL_WAIT_TIME": "594",
-    "ORG_GUEST_COUNT": "5",
-    "OP_GUESTTOBENOTIFIED": "19484",
-    "PerPartyWaitTime": "99",
-    "OP_GUESTNOTIFIEDWAITTIME": "198",
- "GUEST_RANK_MIN": "3",
-  }</t>
   </si>
   <si>
     <t>{clientTimezone: +05:30
@@ -3484,12 +3431,6 @@
     <t>{ "GUEST_RANK_MIN": "1", "TOTAL_WAIT_TIME": "4", "GUEST_AHEAD_COUNT": "0", "ORG_MAX_PARTY": "100", "ORG_WAIT_TIME": "4" }</t>
   </si>
   <si>
-    <t>{ "GUEST_RANK": "1", 
-"TOTAL_WAIT_TIME": "4", 
-"GUEST_AHEAD_COUNT": "0",
-"ORG_WAIT_TIME": "4" }</t>
-  </si>
-  <si>
     <t>{guestId: 19542
 orgId: 83
 templateId: null
@@ -3510,13 +3451,396 @@
     <t>client base is need for creating tiny url</t>
   </si>
   <si>
-    <t>{"serviceResult":{"NOW_SERVING_GUEST_ID":1,"ORG_TOTAL_WAIT_TIME":24,"NEXT_TO_NOTIFY_GUEST_ID":19513,"OP":"ADD","totalWaitTime":24,"nowServingParty":1,"totalPartiesWaiting":5,"orgid":83,"addedGuestId":19514,"guestUUID":"0910c2d2","tinyURL":"https://tinyurl.com/wamax57#/s/0910c2d2","guestRank":5,"languagePrefID":{"langId":1,"langName":"English","languageDisplayName":null,"langIsoCode":"en","active":false},"partyType":-1}</t>
+    <t>{
+    "success": 1,
+    "message": "Organization metrics fetched successfully",
+    "serviceResult": {
+        "notifyUserCount": 10,
+        "orgTotalWaitTime": 25,
+        "orgGuestCount": 0,
+        "guestToBeNotified": "-1",
+        "perPartyWaitTime": 25,
+        "guestNotifiedWaitTime": 250,
+        "guestMinRank": 0
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "success": 1,
+    "message": "Guest metrics fetched successfully",
+    "serviceResult": {
+        "guestRank": null,
+        "totalWaitTime": 25,
+        "guestAheadCount": 0,
+        "orgWaitTime": 25
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "success": 1,
+    "message": "Reset Successfully",
+    "serviceResult": "Reset Successfully"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "success": 1,
+    "message": "guest details fetched Successfully.",
+    "serviceResult": {
+        "guestID": 14096,
+        "organizationID": 2,
+        "name": "Fagun",
+        "uuid": "9d436f9c",
+        "noOfPeople": 1,
+        "noOfChildren": 1,
+        "noOfAdults": 1,
+        "noOfInfants": 1,
+        "partyType": -1,
+        "calloutCount": null,
+        "deviceId": null,
+        "deviceType": null,
+        "sms": "8529637412",
+        "email": null,
+        "prefType": "sms",
+        "optin": 1,
+        "rank": 1,
+        "status": "CHECKIN",
+        "checkinTime": "2017-11-07T11:59:44.000+0000",
+        "seatedTime": null,
+        "createdTime": "2017-11-07T11:59:44.000+0000",
+        "updatedTime": "2020-02-06T13:23:00.000+0000",
+        "incompleteParty": null,
+        "langguagePref": {
+            "langId": 1,
+            "langName": "English",
+            "langIsoCode": "en",
+            "keyName": null,
+            "value": null
+        },
+        "seatingPreference": [
+            {
+                "prefValueId": 41,
+                "prefValue": "First Available",
+                "prefKey": null
+            }
+        ],
+        "marketingPreference": [],
+        "note": "aaa"
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "success": 1,
+    "message": "guest details fetched Successfully.",
+    "serviceResult": {
+        "guestID": 16951,
+        "organizationID": 97,
+        "name": "a",
+        "uuid": "0c2be1e6",
+        "noOfPeople": 20,
+        "noOfChildren": 10,
+        "noOfAdults": 10,
+        "noOfInfants": 0,
+        "partyType": 0,
+        "calloutCount": null,
+        "deviceId": null,
+        "deviceType": null,
+        "sms": "1234567890",
+        "email": null,
+        "prefType": "sms",
+        "optin": 1,
+        "rank": 166,
+        "status": "CHECKIN",
+        "checkinTime": "2019-12-14T11:32:22.000+0000",
+        "seatedTime": null,
+        "createdTime": "2019-12-14T11:32:22.000+0000",
+        "updatedTime": null,
+        "incompleteParty": null,
+        "langguagePref": {
+            "langId": 1,
+            "langName": "English",
+            "langIsoCode": "en",
+            "keyName": null,
+            "value": null
+        },
+        "seatingPreference": [
+            {
+                "prefValueId": 41,
+                "prefValue": "First Available",
+                "prefKey": null
+            }
+        ],
+        "marketingPreference": [],
+        "note": null
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "success": 1,
+    "message": "organization setting updated Successfully.",
+    "serviceResult": {
+        "nowServingParty": 1,
+        "totalWaitTime": 1900,
+        "guestToBeNotified": null,
+        "totalWaitingGuest": 189,
+        "guestNotifiedWaitTime": null,
+        "clientBase": "admin",
+        "perPartyWaitTime": 10,
+        "orgId": 97
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "success": 1,
+    "message": "Sms content fetched successfully",
+    "serviceResult": [
+        {
+            "smsTemplateID": 9,
+            "templateText": "hardik #2: There are 0 parties ahead of you w/ approx. wait-time of 12 min. For LIVE updates:https://tinyurl.com/wamax57#/s/46c2cbd4",
+            "languageID": 1,
+            "level": 1
+        },
+        {
+            "smsTemplateID": 10,
+            "templateText": "hardik #2: Your Table is ALMOST ready. Please make your way back to the restaurant with your entire party and wait for your number to be called. Click for updates: https://tinyurl.com/wamax57#/s/46c2cbd4",
+            "languageID": 1,
+            "level": 2
+        }
+    ]
+}</t>
+  </si>
+  <si>
+    <t>addMarketingPref</t>
+  </si>
+  <si>
+    <t>{
+  "success": 1,
+  "message": "Marketing Preference added successfully.",
+  "serviceResult": "Marketing Preference added successfully"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "success": 1,
+    "message": "guest list fetched Successfully.",
+    "serviceResult": {
+        "totalRecords": 1,
+        "pageNo": 1,
+        "records": [
+            {
+                "guestID": 14096,
+                "organizationID": 2,
+                "name": "Fagun",
+                "uuid": "9d436f9c",
+                "noOfPeople": 1,
+                "noOfChildren": 1,
+                "noOfAdults": 1,
+                "noOfInfants": 1,
+                "partyType": -1,
+                "calloutCount": null,
+                "deviceId": null,
+                "deviceType": null,
+                "sms": "8529637412",
+                "email": null,
+                "prefType": "sms",
+                "optin": 1,
+                "rank": 1,
+                "status": "CHECKIN",
+                "checkinTime": "2017-11-07T11:59:44.000+0000",
+                "seatedTime": null,
+                "createdTime": "2017-11-07T11:59:44.000+0000",
+                "updatedTime": "2020-02-06T13:23:00.000+0000",
+                "incompleteParty": null,
+                "langguagePref": {
+                    "langId": 1,
+                    "langName": "English",
+                    "langIsoCode": "en",
+                    "keyName": null,
+                    "value": null
+                },
+                "seatingPreference": [
+                    {
+                        "prefValueId": 41,
+                        "prefValue": "First Available",
+                        "prefKey": null
+                    }
+                ],
+                "marketingPreference": [],
+                "note": "aaa"
+            }
+        ]
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "success": 1,
+    "message": "guest list fetched Successfully.",
+    "serviceResult": {
+        "totalRecords": 2,
+        "pageNo": 1,
+        "records": [
+            {
+                "guestID": 14096,
+                "organizationID": 2,
+                "name": "Fagun",
+                "uuid": "9d436f9c",
+                "noOfPeople": 1,
+                "noOfChildren": 1,
+                "noOfAdults": 1,
+                "noOfInfants": 1,
+                "partyType": -1,
+                "calloutCount": null,
+                "deviceId": null,
+                "deviceType": null,
+                "sms": "8529637412",
+                "email": null,
+                "prefType": "sms",
+                "optin": 1,
+                "rank": 1,
+                "status": "CHECKIN",
+                "checkinTime": "2017-11-07T11:59:44.000+0000",
+                "seatedTime": null,
+                "createdTime": "2017-11-07T11:59:44.000+0000",
+                "updatedTime": "2020-02-06T13:23:00.000+0000",
+                "incompleteParty": null,
+                "langguagePref": {
+                    "langId": 1,
+                    "langName": "English",
+                    "langIsoCode": "en",
+                    "keyName": null,
+                    "value": null
+                },
+                "seatingPreference": [
+                    {
+                        "prefValueId": 41,
+                        "prefValue": "First Available",
+                        "prefKey": null
+                    }
+                ],
+                "marketingPreference": [],
+                "note": "aaa"
+            },
+            {
+                "guestID": 14099,
+                "organizationID": 2,
+                "name": "Mayur 15th june",
+                "uuid": "dd75c569",
+                "noOfPeople": 15,
+                "noOfChildren": 4,
+                "noOfAdults": 8,
+                "noOfInfants": 3,
+                "partyType": -1,
+                "calloutCount": null,
+                "deviceId": null,
+                "deviceType": null,
+                "sms": "9898989898",
+                "email": null,
+                "prefType": "SMS",
+                "optin": 1,
+                "rank": 2,
+                "status": "CHECKIN",
+                "checkinTime": "2017-11-08T05:52:04.000+0000",
+                "seatedTime": null,
+                "createdTime": "2017-11-08T05:52:04.000+0000",
+                "updatedTime": null,
+                "incompleteParty": null,
+                "langguagePref": {
+                    "langId": 1,
+                    "langName": "English",
+                    "langIsoCode": "en",
+                    "keyName": null,
+                    "value": null
+                },
+                "seatingPreference": [
+                    {
+                        "prefValueId": 39,
+                        "prefValue": "Patio",
+                        "prefKey": null
+                    },
+                    {
+                        "prefValueId": 40,
+                        "prefValue": "Bar",
+                        "prefKey": null
+                    },
+                    {
+                        "prefValueId": 41,
+                        "prefValue": "First Available",
+                        "prefKey": null
+                    }
+                ],
+                "marketingPreference": [
+                    {
+                        "prefValueId": 46,
+                        "prefValue": "Instagram",
+                        "prefKey": null
+                    },
+                    {
+                        "prefValueId": 47,
+                        "prefValue": "Google+",
+                        "prefKey": null
+                    }
+                ],
+                "note": ""
+            }
+        ]
+    }
+}</t>
+  </si>
+  <si>
+    <t>{"orgid":2,"pageSize":2,"pageNo":1}</t>
+  </si>
+  <si>
+    <t>{"orgid":2,searchtext:"fagun","pageSize":2,"pageNo":1}</t>
+  </si>
+  <si>
+    <t>{
+    "success": 1,
+    "message": "guest details updated Successfully.",
+    "serviceResult": {
+        "nowServingGuestId": 0,
+        "nextToNotifyGuestId": -1,
+        "op": "UPDATE",
+        "totalWaitTime": 25,
+        "totalGuestWaiting": 0,
+        "orgId": 83,
+        "addedGuestId": 18776,
+        "guestUUID": null,
+        "tinyURL": "https://tinyurl.com/wamax57#/s/string",
+        "guestRank": null,
+        "languagePref": {
+            "langId": 1,
+            "langName": "English",
+            "langIsoCode": "en",
+            "keyName": "string",
+            "value": "string"
+        },
+        "clientBase": "admin"
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+  "guestID": 14099,
+  "marketingPreference": [
+    {
+      "prefKey": null,
+      "prefValue": "Facebook",
+      "prefValueId":45
+    }
+  ]
+}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3637,7 +3961,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -3810,11 +4134,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3848,12 +4209,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3909,6 +4264,66 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4189,10 +4604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4227,393 +4642,393 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="52" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="31" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>100</v>
+      <c r="F2" s="60" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="2" customFormat="1" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34" t="s">
+      <c r="B3" s="32"/>
+      <c r="C3" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="F3" s="37" t="s">
-        <v>106</v>
+      <c r="E3" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" s="2" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34" t="s">
+      <c r="B4" s="32"/>
+      <c r="C4" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="32" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="34" t="s">
-        <v>14</v>
+      <c r="F4" s="59" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="175.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="E5" s="32" t="s">
+      <c r="D5" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="32" t="s">
-        <v>81</v>
+      <c r="F5" s="30" t="s">
+        <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="218.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30" t="s">
+    <row r="6" spans="1:6" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="E6" s="32" t="s">
+      <c r="D6" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="32" t="s">
-        <v>80</v>
+      <c r="F6" s="30" t="s">
+        <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="218.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30" t="s">
+    <row r="7" spans="1:6" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="28" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="32" t="s">
-        <v>79</v>
+      <c r="F7" s="54" t="s">
+        <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="205.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="30" t="s">
+    <row r="8" spans="1:6" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="38" t="s">
-        <v>82</v>
+      <c r="F8" s="36" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="126.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="E9" s="53" t="s">
+      <c r="D9" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="31" t="s">
-        <v>83</v>
+      <c r="F9" s="29" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="31" t="s">
+      <c r="B10" s="28"/>
+      <c r="C10" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="31" t="s">
-        <v>101</v>
+      <c r="D10" s="29" t="s">
+        <v>94</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="31" t="s">
-        <v>84</v>
+      <c r="F10" s="29" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="4" customFormat="1" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="40" t="s">
-        <v>94</v>
-      </c>
-      <c r="F11" s="40" t="s">
-        <v>94</v>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" s="38" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="5" customFormat="1" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
     </row>
     <row r="13" spans="1:6" s="5" customFormat="1" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
       <c r="E13" s="19"/>
-      <c r="F13" s="20"/>
+      <c r="F13" s="37"/>
     </row>
     <row r="14" spans="1:6" ht="199.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="B14" s="30" t="s">
+      <c r="A14" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="E14" s="31" t="s">
+      <c r="D14" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="31" t="s">
-        <v>111</v>
+      <c r="F14" s="55" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="5" customFormat="1" ht="240" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="37" t="s">
         <v>47</v>
       </c>
       <c r="C15" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="42" t="s">
-        <v>85</v>
+      <c r="D15" s="40" t="s">
+        <v>81</v>
       </c>
       <c r="E15" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="40" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="190.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+    </row>
+    <row r="17" spans="1:6" s="1" customFormat="1" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="B16" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-    </row>
-    <row r="17" spans="1:6" s="1" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="46" t="s">
-        <v>102</v>
-      </c>
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="55" t="s">
+      <c r="C17" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="F17" s="44" t="s">
-        <v>87</v>
+      <c r="E17" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="42" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="5" customFormat="1" ht="154.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="37" t="s">
         <v>45</v>
       </c>
       <c r="D18" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="42" t="s">
+      <c r="E18" s="40" t="s">
         <v>51</v>
       </c>
       <c r="F18" s="20"/>
     </row>
     <row r="19" spans="1:6" s="5" customFormat="1" ht="71.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="E19" s="42" t="s">
+      <c r="D19" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="40" t="s">
         <v>62</v>
       </c>
       <c r="F19" s="20"/>
     </row>
     <row r="20" spans="1:6" s="5" customFormat="1" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="37" t="s">
         <v>52</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="42" t="s">
-        <v>88</v>
+      <c r="D20" s="40" t="s">
+        <v>84</v>
       </c>
       <c r="E20" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="F20" s="20"/>
+      <c r="F20" s="37"/>
     </row>
     <row r="21" spans="1:6" s="5" customFormat="1" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="39" t="s">
+      <c r="B21" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="39" t="s">
+      <c r="C21" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="39" t="s">
+      <c r="D21" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="42" t="s">
+      <c r="E21" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="F21" s="39"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" spans="1:6" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
       <c r="E22" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="F22" s="43" t="s">
-        <v>89</v>
+        <v>85</v>
+      </c>
+      <c r="F22" s="41" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="2" customFormat="1" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="34"/>
+      <c r="B23" s="32"/>
       <c r="C23" s="9" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>59</v>
@@ -4622,118 +5037,166 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="3" customFormat="1" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="45" t="s">
+    <row r="24" spans="1:6" s="3" customFormat="1" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45" t="s">
+      <c r="B24" s="43"/>
+      <c r="C24" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="45" t="s">
+      <c r="D24" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="23" t="s">
+      <c r="E24" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="24" t="s">
-        <v>69</v>
+      <c r="F24" s="45" t="s">
+        <v>109</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="1" customFormat="1" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="46" t="s">
+    <row r="25" spans="1:6" s="1" customFormat="1" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="46" t="s">
-        <v>110</v>
-      </c>
-      <c r="C25" s="44" t="s">
+      <c r="B25" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="44" t="s">
+      <c r="D25" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="E25" s="75" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="E25" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="F25" s="46"/>
     </row>
     <row r="26" spans="1:6" s="3" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="45" t="s">
+      <c r="A26" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="B26" s="45"/>
-      <c r="C26" s="47" t="s">
+      <c r="B26" s="43"/>
+      <c r="C26" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="47" t="s">
+      <c r="D26" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="E26" s="45"/>
-      <c r="F26" s="25"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="23"/>
     </row>
     <row r="27" spans="1:6" s="7" customFormat="1" ht="154.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="48" t="s">
+      <c r="A27" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="48"/>
-      <c r="C27" s="48" t="s">
+      <c r="B27" s="46"/>
+      <c r="C27" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="D27" s="48" t="s">
+      <c r="D27" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="E27" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="F27" s="50" t="s">
-        <v>86</v>
+      <c r="E27" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" s="48" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="46" t="s">
+      <c r="A28" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="B28" s="46"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="52"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="50"/>
     </row>
-    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="26"/>
-      <c r="B29" s="27" t="s">
+    <row r="29" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="66" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="69"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="64"/>
+      <c r="E29" s="72" t="s">
+        <v>117</v>
+      </c>
+      <c r="F29" s="56" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="67"/>
+      <c r="B30" s="70"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="73"/>
+      <c r="F30" s="57"/>
+    </row>
+    <row r="31" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="67"/>
+      <c r="B31" s="70"/>
+      <c r="C31" s="65"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="73"/>
+      <c r="F31" s="57"/>
+    </row>
+    <row r="32" spans="1:6" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="68"/>
+      <c r="B32" s="71"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="74"/>
+      <c r="F32" s="58"/>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="24"/>
+      <c r="B33" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="29"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="27"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="6" t="s">
-        <v>96</v>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="6" t="s">
+        <v>90</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="5" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="F29:F32"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="B29:B32"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
- update waitlist doc for sms API responses
</commit_message>
<xml_diff>
--- a/doc/WaitlistAPIListTechRevamp.xlsx
+++ b/doc/WaitlistAPIListTechRevamp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Kyobee11Nov\NewUI branch\RevisedKyobee\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ria\Kyobee\Kyobee\RevisedKyobee\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="131">
   <si>
     <t>API</t>
   </si>
@@ -157,9 +157,6 @@
     <t>guestId:19504,orgId:83,templateId:null,smsContent:"Fagun #1: There are 0 parties ahead of you w/ approx. wait-time of 6 min. For LIVE updates:https://tinyurl.com/wamax57#/s/2d65c97f",metrics:null,templateLevel:1</t>
   </si>
   <si>
-    <t>{"status":"SUCCESS","errorCode":null,"errorDescription":"SUCCESS","serviceResponseDescription":null,"serviceIdentifier":null,"serviceResult":null,"serviceResultSms":null}</t>
-  </si>
-  <si>
     <t>guestID:19504,organizationID:83,name:"Fagun",note:null,uuid:"2d65c97f",noOfChildren:0,noOfAdults:1,noOfInfants:0,noOfPeople:1,quoteTime:0,partyType:-1,email:null,sms:"4242423423",status:"CHECKIN",rank:1,prefType:"sms",guestPreferences:null,guestMarketingPreferences:null,optin:true,calloutCount:null,checkinTime:1580291488000,seatedTime:null,createdTime:1580301769170,updatedTime:1580301769170,incompleteParty:null,seatingPreference:"",marketingPreference:"Instagram",deviceType:null,deviceId:null,languagePref:{langId:1,langName:"English",languageDisplayName:"English",langIsoCode:"en",active:true}</t>
   </si>
   <si>
@@ -192,9 +189,6 @@
       "levelDesc": "Check-in",
       "languageID": 1
     }]</t>
-  </si>
-  <si>
-    <t>fetchSmsContent</t>
   </si>
   <si>
     <t>orgId:83,guestId:19514,guestName:"w435345",langId:1,tempLevel:3,gusetRank:5,clientBase:"admin",guestUuid:"0910c2d2"</t>
@@ -328,18 +322,6 @@
 smsContent: "nhh #1: There are 0 parties ahead of you w/ approx. wait-time of 1 min. For LIVE updates:https://tinyurl.com/wamax57#/s/3be4cbe3"
 metrics: null
 templateLevel: 1}</t>
-  </si>
-  <si>
-    <t>guestId: 19542
-orgId: 83
-smsContent: "nhh #1: There are 0 parties ahead of you w/ approx. wait-time of 1 min. For LIVE updates:https://tinyurl.com/wamax57#/s/3be4cbe3"
-templateLevel: 1</t>
-  </si>
-  <si>
-    <t>orgId:83,guestId:19514,guestName:"w435345",gusetRank:5,guestUuid:"0910c2d2",langId:1,clientBase</t>
-  </si>
-  <si>
-    <t>client base is need for creating tiny url</t>
   </si>
   <si>
     <t>{
@@ -4736,12 +4718,68 @@
     <t xml:space="preserve">http://44.232.86.255:8111/rest/waitlist/refreshLanguage
 </t>
   </si>
+  <si>
+    <t>fetchSmsContent(smsContent)</t>
+  </si>
+  <si>
+    <t>{
+"guestName":"hardik",
+"guestId":14464,
+"guestRank":2,
+"guestUuid":"46c2cbd4",
+"langId":1,
+"orgId": 16,
+"clientBase":"admin"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "success": 1,
+    "message": "Sms content fetched successfully",
+    "serviceResult": [
+        {
+            "smsTemplateID": 9,
+            "templateText": "hardik #2: There are 1 parties ahead of you w/ approx. wait-time of 24 min. For LIVE updates:https://tinyurl.com/wamax57#/s/46c2cbd4",
+            "languageID": 1,
+            "level": 1
+        },
+        {
+            "smsTemplateID": 10,
+            "templateText": "hardik #2: Your Table is ALMOST ready. Please make your way back to the restaurant with your entire party and wait for your number to be called. Click for updates: https://tinyurl.com/wamax57#/s/46c2cbd4",
+            "languageID": 1,
+            "level": 2
+        }
+    ]
+}</t>
+  </si>
+  <si>
+    <t>http://44.232.86.255:8111/rest/waitlist/guest/organizationTemplate/smsContent</t>
+  </si>
+  <si>
+    <t>{
+  "success": 1,
+  "message": "Sms sent successfully",
+  "serviceResult": "Sms sent successfully"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "guestId": 14096,
+  "orgId": 2,
+  "smsContent": null,
+  "templateId": 0,
+  "templateLevel": 1
+}</t>
+  </si>
+  <si>
+    <t>http://44.232.86.255:8111/rest/waitlist/sendSMS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="26" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4780,13 +4818,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B0F0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -5179,9 +5210,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -5191,168 +5222,177 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5637,8 +5677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:A32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5674,30 +5714,30 @@
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" ht="205.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="78" t="s">
+      <c r="D2" s="63" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="21" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="2" customFormat="1" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>8</v>
@@ -5706,18 +5746,18 @@
         <v>8</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="2" customFormat="1" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C4" s="23" t="s">
         <v>9</v>
@@ -5729,7 +5769,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="175.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5737,19 +5777,19 @@
         <v>11</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E5" s="30" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="14" customFormat="1" ht="200.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5757,27 +5797,27 @@
         <v>12</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="200.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="72" t="s">
-        <v>104</v>
+      <c r="B7" s="60" t="s">
+        <v>99</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>16</v>
@@ -5789,7 +5829,7 @@
         <v>17</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="200.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5797,7 +5837,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>21</v>
@@ -5809,7 +5849,7 @@
         <v>20</v>
       </c>
       <c r="F8" s="31" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="138" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5817,44 +5857,44 @@
         <v>19</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="200.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="4" customFormat="1" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="34" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B11" s="34" t="s">
         <v>30</v>
@@ -5862,15 +5902,15 @@
       <c r="C11" s="34"/>
       <c r="D11" s="34"/>
       <c r="E11" s="35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F11" s="35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="5" customFormat="1" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="36" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B12" s="36" t="s">
         <v>24</v>
@@ -5882,7 +5922,7 @@
     </row>
     <row r="13" spans="1:6" s="5" customFormat="1" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="36" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B13" s="36" t="s">
         <v>24</v>
@@ -5894,68 +5934,68 @@
     </row>
     <row r="14" spans="1:6" ht="199.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="B14" s="73" t="s">
-        <v>114</v>
+        <v>105</v>
+      </c>
+      <c r="B14" s="61" t="s">
+        <v>109</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E14" s="38" t="s">
         <v>26</v>
       </c>
       <c r="F14" s="39" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="199.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="E15" s="72" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="60" t="s">
         <v>27</v>
       </c>
       <c r="F15" s="39" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="190.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>25</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="11" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="1" customFormat="1" ht="200.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="42" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B17" s="44" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C17" s="43" t="s">
         <v>28</v>
@@ -5964,15 +6004,15 @@
         <v>28</v>
       </c>
       <c r="E17" s="44" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F17" s="44" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="5" customFormat="1" ht="154.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="36" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B18" s="36" t="s">
         <v>32</v>
@@ -5990,43 +6030,43 @@
     </row>
     <row r="19" spans="1:6" s="5" customFormat="1" ht="71.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="36" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B19" s="36" t="s">
         <v>29</v>
       </c>
       <c r="C19" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="41" t="s">
         <v>37</v>
-      </c>
-      <c r="D19" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="41" t="s">
-        <v>38</v>
       </c>
       <c r="F19" s="45"/>
     </row>
     <row r="20" spans="1:6" s="5" customFormat="1" ht="237" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="36" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B20" s="37" t="s">
         <v>29</v>
       </c>
       <c r="C20" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" s="41" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E20" s="40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F20" s="36"/>
     </row>
     <row r="21" spans="1:6" s="5" customFormat="1" ht="189.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="36" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B21" s="36" t="s">
         <v>29</v>
@@ -6038,13 +6078,13 @@
         <v>8</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" s="77"/>
+        <v>40</v>
+      </c>
+      <c r="F21" s="62"/>
     </row>
     <row r="22" spans="1:6" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="46" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B22" s="34" t="s">
         <v>33</v>
@@ -6052,187 +6092,189 @@
       <c r="C22" s="34"/>
       <c r="D22" s="34"/>
       <c r="E22" s="47" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F22" s="48" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="2" customFormat="1" ht="158.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="23"/>
+      <c r="B23" s="86" t="s">
+        <v>130</v>
+      </c>
       <c r="C23" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="D23" s="85" t="s">
+        <v>129</v>
       </c>
       <c r="E23" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F23" s="21" t="s">
-        <v>36</v>
+      <c r="F23" s="85" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="3" customFormat="1" ht="200.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24" s="49"/>
       <c r="C24" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="50" t="s">
-        <v>45</v>
-      </c>
       <c r="F24" s="50" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="1" customFormat="1" ht="200.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="84" t="s">
+        <v>125</v>
+      </c>
+      <c r="E25" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="42" t="s">
-        <v>75</v>
-      </c>
-      <c r="C25" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="44" t="s">
-        <v>74</v>
-      </c>
-      <c r="E25" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="44" t="s">
-        <v>79</v>
+      <c r="F25" s="51" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="3" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="49" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B26" s="49"/>
       <c r="C26" s="50" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D26" s="50" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E26" s="49"/>
       <c r="F26" s="52"/>
     </row>
     <row r="27" spans="1:6" s="7" customFormat="1" ht="200.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C27" s="53" t="s">
-        <v>53</v>
-      </c>
       <c r="D27" s="53" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E27" s="54" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F27" s="55" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="1" customFormat="1" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="42" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="C28" s="79"/>
+        <v>123</v>
+      </c>
+      <c r="C28" s="64"/>
       <c r="D28" s="42"/>
-      <c r="E28" s="80"/>
+      <c r="E28" s="65"/>
       <c r="F28" s="44" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="56" t="s">
-        <v>80</v>
+      <c r="A29" s="66" t="s">
+        <v>75</v>
       </c>
       <c r="B29" s="81" t="s">
-        <v>126</v>
-      </c>
-      <c r="C29" s="57"/>
-      <c r="D29" s="58"/>
-      <c r="E29" s="59" t="s">
-        <v>84</v>
-      </c>
-      <c r="F29" s="74" t="s">
-        <v>81</v>
+        <v>121</v>
+      </c>
+      <c r="C29" s="78"/>
+      <c r="D29" s="75"/>
+      <c r="E29" s="72" t="s">
+        <v>79</v>
+      </c>
+      <c r="F29" s="69" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="60"/>
+      <c r="A30" s="67"/>
       <c r="B30" s="82"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="63"/>
-      <c r="F30" s="75"/>
+      <c r="C30" s="79"/>
+      <c r="D30" s="76"/>
+      <c r="E30" s="73"/>
+      <c r="F30" s="70"/>
     </row>
     <row r="31" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="60"/>
+      <c r="A31" s="67"/>
       <c r="B31" s="82"/>
-      <c r="C31" s="61"/>
-      <c r="D31" s="62"/>
-      <c r="E31" s="63"/>
-      <c r="F31" s="75"/>
+      <c r="C31" s="79"/>
+      <c r="D31" s="76"/>
+      <c r="E31" s="73"/>
+      <c r="F31" s="70"/>
     </row>
     <row r="32" spans="1:6" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="64"/>
+      <c r="A32" s="68"/>
       <c r="B32" s="83"/>
-      <c r="C32" s="65"/>
-      <c r="D32" s="66"/>
-      <c r="E32" s="67"/>
-      <c r="F32" s="76"/>
+      <c r="C32" s="80"/>
+      <c r="D32" s="77"/>
+      <c r="E32" s="74"/>
+      <c r="F32" s="71"/>
     </row>
     <row r="33" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="68"/>
-      <c r="B33" s="69" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="70"/>
-      <c r="D33" s="70"/>
-      <c r="E33" s="70"/>
-      <c r="F33" s="71"/>
+      <c r="A33" s="56"/>
+      <c r="B33" s="57" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="58"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="59"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B42" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -6248,7 +6290,7 @@
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5"/>
+    <hyperlink ref="B5" display="Name changed to fetchGuestList, can we not remove pageReqParam,Need to remove guestPreferences from table as well as response,need to remove createdby,updatedBy,createdAt,updatedAt,guestPreferenceMap and ,guestMarketingPreferences are seating pre and mark"/>
     <hyperlink ref="B27" r:id="rId4"/>
     <hyperlink ref="B10" r:id="rId5"/>
     <hyperlink ref="B14" r:id="rId6" display="http://44.232.86.255:8111/rest/waitlist/guest/"/>
@@ -6256,8 +6298,10 @@
     <hyperlink ref="B16" r:id="rId8"/>
     <hyperlink ref="B29" r:id="rId9"/>
     <hyperlink ref="B28" r:id="rId10"/>
+    <hyperlink ref="B25" r:id="rId11"/>
+    <hyperlink ref="B23" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>